<commit_message>
added python 3 support only for Landsat images
</commit_message>
<xml_diff>
--- a/docs/InputEXCEL_v3_3_7.xlsx
+++ b/docs/InputEXCEL_v3_3_7.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tih\Documents\Water_Accounting\GitHub\SEBAL\SEBAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PySebal\PySEBAL_Pareeth\PySEBAL_dev\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5748" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General_Input" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>InputMap</t>
   </si>
@@ -239,70 +239,22 @@
     <t>MOD09GA.A2008129.h18v05.006.2015173152648</t>
   </si>
   <si>
-    <t>LC81770392016167LGN00</t>
-  </si>
-  <si>
-    <t>LC81770392016167LGN01</t>
-  </si>
-  <si>
     <t>VIIRS_SVIO5_npp_d20160615_t1142431_e1148235_b24007_c20160615174824617353_noaa_ops.tif</t>
   </si>
   <si>
     <t>PROBAV_S5_TOC_X21Y04_20160621_100M_V001</t>
   </si>
   <si>
-    <t>$HOME\Input\Landsat</t>
-  </si>
-  <si>
-    <t>$HOME\Output\LS</t>
-  </si>
-  <si>
-    <t>$HOME\Input\DEM\DEM_HydroShed_m_LS.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\VIIRS-PROBAV</t>
-  </si>
-  <si>
-    <t>$HOME\Output\VIIRS_PROBAV</t>
-  </si>
-  <si>
-    <t>$HOME\Input\DEM\DEM_HydroShed_m_VIIRS.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Meteo\three_hourly\avgsurft_inst\T_GLDAS-NOAH_C_3hour_2016.06.15_4.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Meteo\daily\avgsurft_inst\mean\T_GLDAS-NOAH_C_daily_2016.06.15.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Meteo\three_hourly\Hum_Calculated\Humidity_percentage_Calculated_4.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Meteo\daily\Hum_Calculated\Humidity_percentage_Calculated_daily.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Meteo\three_hourly\wind_f_inst\W_GLDAS-NOAH_m-s-1_3hour_2016.06.15_4.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Meteo\daily\wind_f_inst\mean\W_GLDAS-NOAH_m-s-1_daily_2016.06.15.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Meteo\daily\swdown_f_tavg\mean\SWdown_GLDAS-NOAH_W-m-2_daily_2016.06.15.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Meteo\three_hourly\swdown_f_tavg\SWdown_GLDAS-NOAH_W-m-2_3hour_2016.06.15_4.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Soils\wcsat_topsoil.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Soils\wcsat_subsoil.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Soils\wcpf2_topsoil.tif</t>
-  </si>
-  <si>
-    <t>$HOME\Input\Soils\wcpf4.2_topsoil.tif</t>
+    <t>D:\PySebal\test_data\input\insat</t>
+  </si>
+  <si>
+    <t>D:\PySebal\test_data\output</t>
+  </si>
+  <si>
+    <t>LC08_L1TP_173049_20140310_20170425_01_T1</t>
+  </si>
+  <si>
+    <t>D:\PySebal\test_data\input\dem_dal.tif</t>
   </si>
 </sst>
 </file>
@@ -743,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,16 +734,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>35</v>
@@ -800,18 +752,6 @@
     <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>33</v>
@@ -951,9 +891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1067,48 +1005,20 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="4">
-        <v>2</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="L3" s="4">
-        <v>1</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="N3" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="O3" s="4">
-        <v>0.4</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
       <c r="R3" s="7" t="s">
         <v>33</v>
       </c>
@@ -1231,7 +1141,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1308,30 +1218,14 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="4">
-        <v>2.5</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -1438,14 +1332,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.77734375" bestFit="1" customWidth="1"/>
@@ -1478,7 +1372,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4">
         <v>8</v>
@@ -1500,21 +1394,11 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="4">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.5</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="J3" s="7" t="s">
         <v>33</v>
       </c>
@@ -1644,11 +1528,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" s="4">
         <v>2</v>
@@ -1668,11 +1552,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E3" s="4">
         <v>2</v>

</xml_diff>